<commit_message>
feat: Add google sheets for saving the data online
</commit_message>
<xml_diff>
--- a/live_crypto_data.xlsx
+++ b/live_crypto_data.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98448</v>
+        <v>98411</v>
       </c>
       <c r="D2" t="n">
-        <v>1951373082879</v>
+        <v>1950132842535</v>
       </c>
       <c r="E2" t="n">
-        <v>33715408965</v>
+        <v>33488025597</v>
       </c>
       <c r="F2" t="n">
-        <v>1.33457</v>
+        <v>1.24586</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2721.08</v>
+        <v>2717.24</v>
       </c>
       <c r="D3" t="n">
-        <v>327894112535</v>
+        <v>327567292210</v>
       </c>
       <c r="E3" t="n">
-        <v>17393359029</v>
+        <v>17379584261</v>
       </c>
       <c r="F3" t="n">
-        <v>3.18075</v>
+        <v>2.99203</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +528,13 @@
         <v>2.52</v>
       </c>
       <c r="D4" t="n">
-        <v>145651511241</v>
+        <v>145396047436</v>
       </c>
       <c r="E4" t="n">
-        <v>3884560995</v>
+        <v>3895982591</v>
       </c>
       <c r="F4" t="n">
-        <v>5.34548</v>
+        <v>4.81415</v>
       </c>
     </row>
     <row r="5">
@@ -552,13 +552,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>141900653641</v>
+        <v>141898810750</v>
       </c>
       <c r="E5" t="n">
-        <v>65102801679</v>
+        <v>64686637587</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0032</v>
+        <v>0.00393</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>205.79</v>
+        <v>205.16</v>
       </c>
       <c r="D6" t="n">
-        <v>100418630362</v>
+        <v>100083961971</v>
       </c>
       <c r="E6" t="n">
-        <v>4687316453</v>
+        <v>4684942856</v>
       </c>
       <c r="F6" t="n">
-        <v>1.35311</v>
+        <v>0.99521</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>639.5599999999999</v>
+        <v>637.47</v>
       </c>
       <c r="D7" t="n">
-        <v>93338152115</v>
+        <v>92962391635</v>
       </c>
       <c r="E7" t="n">
-        <v>1189117433</v>
+        <v>1194563777</v>
       </c>
       <c r="F7" t="n">
-        <v>5.28026</v>
+        <v>4.67356</v>
       </c>
     </row>
     <row r="8">
@@ -624,13 +624,13 @@
         <v>0.999996</v>
       </c>
       <c r="D8" t="n">
-        <v>56257173589</v>
+        <v>56257179127</v>
       </c>
       <c r="E8" t="n">
-        <v>4664120576</v>
+        <v>4785194982</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00447</v>
+        <v>0.00341</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.268759</v>
+        <v>0.26772</v>
       </c>
       <c r="D9" t="n">
-        <v>39756009209</v>
+        <v>39645674838</v>
       </c>
       <c r="E9" t="n">
-        <v>1339590691</v>
+        <v>1351418423</v>
       </c>
       <c r="F9" t="n">
-        <v>7.48173</v>
+        <v>6.91197</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.79686</v>
+        <v>0.795423</v>
       </c>
       <c r="D10" t="n">
-        <v>28609148597</v>
+        <v>28535539546</v>
       </c>
       <c r="E10" t="n">
-        <v>1149078210</v>
+        <v>1157591917</v>
       </c>
       <c r="F10" t="n">
-        <v>15.16938</v>
+        <v>14.58889</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2720.11</v>
+        <v>2716.6</v>
       </c>
       <c r="D11" t="n">
-        <v>25565844331</v>
+        <v>25553871100</v>
       </c>
       <c r="E11" t="n">
-        <v>62340505</v>
+        <v>62729785</v>
       </c>
       <c r="F11" t="n">
-        <v>3.19065</v>
+        <v>3.07224</v>
       </c>
     </row>
     <row r="12">
@@ -717,16 +717,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.245671</v>
+        <v>0.246416</v>
       </c>
       <c r="D12" t="n">
-        <v>21152017122</v>
+        <v>21201842858</v>
       </c>
       <c r="E12" t="n">
-        <v>829372203</v>
+        <v>829560532</v>
       </c>
       <c r="F12" t="n">
-        <v>5.86361</v>
+        <v>5.871</v>
       </c>
     </row>
     <row r="13">
@@ -741,16 +741,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>98243</v>
+        <v>98186</v>
       </c>
       <c r="D13" t="n">
-        <v>12682086754</v>
+        <v>12678178802</v>
       </c>
       <c r="E13" t="n">
-        <v>427682725</v>
+        <v>388622667</v>
       </c>
       <c r="F13" t="n">
-        <v>1.34863</v>
+        <v>1.24356</v>
       </c>
     </row>
     <row r="14">
@@ -765,16 +765,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>19.74</v>
+        <v>19.69</v>
       </c>
       <c r="D14" t="n">
-        <v>12590031478</v>
+        <v>12564995949</v>
       </c>
       <c r="E14" t="n">
-        <v>548482490</v>
+        <v>544695835</v>
       </c>
       <c r="F14" t="n">
-        <v>6.35381</v>
+        <v>5.8177</v>
       </c>
     </row>
     <row r="15">
@@ -789,16 +789,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3238.84</v>
+        <v>3239.85</v>
       </c>
       <c r="D15" t="n">
-        <v>11039148061</v>
+        <v>11043842730</v>
       </c>
       <c r="E15" t="n">
-        <v>64817497</v>
+        <v>58085274</v>
       </c>
       <c r="F15" t="n">
-        <v>3.24604</v>
+        <v>3.09269</v>
       </c>
     </row>
     <row r="16">
@@ -813,16 +813,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>26.7</v>
+        <v>26.69</v>
       </c>
       <c r="D16" t="n">
-        <v>10994919336</v>
+        <v>10989021026</v>
       </c>
       <c r="E16" t="n">
-        <v>331714933</v>
+        <v>331081392</v>
       </c>
       <c r="F16" t="n">
-        <v>6.00946</v>
+        <v>5.86355</v>
       </c>
     </row>
     <row r="17">
@@ -837,16 +837,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.53</v>
+        <v>3.52</v>
       </c>
       <c r="D17" t="n">
-        <v>10912906068</v>
+        <v>10870593863</v>
       </c>
       <c r="E17" t="n">
-        <v>1427570706</v>
+        <v>1509548477</v>
       </c>
       <c r="F17" t="n">
-        <v>14.1617</v>
+        <v>12.90979</v>
       </c>
     </row>
     <row r="18">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.337276</v>
+        <v>0.333881</v>
       </c>
       <c r="D18" t="n">
-        <v>10318534341</v>
+        <v>10215378436</v>
       </c>
       <c r="E18" t="n">
-        <v>324922947</v>
+        <v>330524272</v>
       </c>
       <c r="F18" t="n">
-        <v>7.91314</v>
+        <v>6.59628</v>
       </c>
     </row>
     <row r="19">
@@ -885,16 +885,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>129.3</v>
+        <v>129.46</v>
       </c>
       <c r="D19" t="n">
-        <v>9762972982</v>
+        <v>9759833253</v>
       </c>
       <c r="E19" t="n">
-        <v>1910665295</v>
+        <v>1918231053</v>
       </c>
       <c r="F19" t="n">
-        <v>14.1042</v>
+        <v>14.06198</v>
       </c>
     </row>
     <row r="20">
@@ -909,16 +909,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.88</v>
+        <v>3.87</v>
       </c>
       <c r="D20" t="n">
-        <v>9672293895</v>
+        <v>9650081360</v>
       </c>
       <c r="E20" t="n">
-        <v>130607992</v>
+        <v>132078117</v>
       </c>
       <c r="F20" t="n">
-        <v>1.21309</v>
+        <v>1.06107</v>
       </c>
     </row>
     <row r="21">
@@ -933,16 +933,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.637e-05</v>
+        <v>1.638e-05</v>
       </c>
       <c r="D21" t="n">
-        <v>9641221964</v>
+        <v>9641835463</v>
       </c>
       <c r="E21" t="n">
-        <v>207651538</v>
+        <v>211243492</v>
       </c>
       <c r="F21" t="n">
-        <v>3.56651</v>
+        <v>3.16442</v>
       </c>
     </row>
     <row r="22">
@@ -957,16 +957,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.248038</v>
+        <v>0.246595</v>
       </c>
       <c r="D22" t="n">
-        <v>9493433882</v>
+        <v>9434503192</v>
       </c>
       <c r="E22" t="n">
-        <v>292432253</v>
+        <v>291583721</v>
       </c>
       <c r="F22" t="n">
-        <v>4.89133</v>
+        <v>3.76763</v>
       </c>
     </row>
     <row r="23">
@@ -984,13 +984,13 @@
         <v>9.9</v>
       </c>
       <c r="D23" t="n">
-        <v>9147247276</v>
+        <v>9144770423</v>
       </c>
       <c r="E23" t="n">
-        <v>260014</v>
+        <v>260436</v>
       </c>
       <c r="F23" t="n">
-        <v>0.04176</v>
+        <v>0.03344</v>
       </c>
     </row>
     <row r="24">
@@ -1005,16 +1005,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="D24" t="n">
-        <v>8371354818</v>
+        <v>8370764279</v>
       </c>
       <c r="E24" t="n">
-        <v>5961431</v>
+        <v>5957558</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.00542</v>
+        <v>0.19937</v>
       </c>
     </row>
     <row r="25">
@@ -1029,16 +1029,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>24.77</v>
+        <v>24.66</v>
       </c>
       <c r="D25" t="n">
-        <v>8260040006</v>
+        <v>8243173619</v>
       </c>
       <c r="E25" t="n">
-        <v>116232846</v>
+        <v>115989134</v>
       </c>
       <c r="F25" t="n">
-        <v>5.41718</v>
+        <v>4.31436</v>
       </c>
     </row>
     <row r="26">
@@ -1053,16 +1053,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2720.02</v>
+        <v>2717.2</v>
       </c>
       <c r="D26" t="n">
-        <v>7927950602</v>
+        <v>7937252033</v>
       </c>
       <c r="E26" t="n">
-        <v>993409861</v>
+        <v>885393927</v>
       </c>
       <c r="F26" t="n">
-        <v>3.21846</v>
+        <v>3.00492</v>
       </c>
     </row>
     <row r="27">
@@ -1077,16 +1077,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5.2</v>
+        <v>5.16</v>
       </c>
       <c r="D27" t="n">
-        <v>7908444620</v>
+        <v>7861278815</v>
       </c>
       <c r="E27" t="n">
-        <v>229647938</v>
+        <v>231265903</v>
       </c>
       <c r="F27" t="n">
-        <v>8.13523</v>
+        <v>7.32178</v>
       </c>
     </row>
     <row r="28">
@@ -1101,16 +1101,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6.46</v>
+        <v>6.45</v>
       </c>
       <c r="D28" t="n">
-        <v>7748553696</v>
+        <v>7743984697</v>
       </c>
       <c r="E28" t="n">
-        <v>281063193</v>
+        <v>279334002</v>
       </c>
       <c r="F28" t="n">
-        <v>0.69833</v>
+        <v>0.80524</v>
       </c>
     </row>
     <row r="29">
@@ -1125,16 +1125,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>343.7</v>
+        <v>341.87</v>
       </c>
       <c r="D29" t="n">
-        <v>6815265994</v>
+        <v>6777263500</v>
       </c>
       <c r="E29" t="n">
-        <v>153486945</v>
+        <v>152775061</v>
       </c>
       <c r="F29" t="n">
-        <v>4.76934</v>
+        <v>3.92785</v>
       </c>
     </row>
     <row r="30">
@@ -1149,16 +1149,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0.9997819999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>6051770168</v>
+        <v>6051454969</v>
       </c>
       <c r="E30" t="n">
-        <v>110916685</v>
+        <v>112005820</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.02086</v>
+        <v>-0.02404</v>
       </c>
     </row>
     <row r="31">
@@ -1173,16 +1173,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>10.02</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>6013532369</v>
+        <v>5994229870</v>
       </c>
       <c r="E31" t="n">
-        <v>297342254</v>
+        <v>299220810</v>
       </c>
       <c r="F31" t="n">
-        <v>9.618930000000001</v>
+        <v>9.119400000000001</v>
       </c>
     </row>
     <row r="32">
@@ -1197,16 +1197,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5.95</v>
+        <v>5.93</v>
       </c>
       <c r="D32" t="n">
-        <v>5779201809</v>
+        <v>5766880575</v>
       </c>
       <c r="E32" t="n">
-        <v>224092217</v>
+        <v>222727811</v>
       </c>
       <c r="F32" t="n">
-        <v>-2.87862</v>
+        <v>-3.07645</v>
       </c>
     </row>
     <row r="33">
@@ -1221,16 +1221,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2875.1</v>
+        <v>2877.61</v>
       </c>
       <c r="D33" t="n">
-        <v>5467936915</v>
+        <v>5471967311</v>
       </c>
       <c r="E33" t="n">
-        <v>14418100</v>
+        <v>15121965</v>
       </c>
       <c r="F33" t="n">
-        <v>2.88959</v>
+        <v>3.04936</v>
       </c>
     </row>
     <row r="34">
@@ -1245,16 +1245,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="D34" t="n">
-        <v>4456657456</v>
+        <v>4429222888</v>
       </c>
       <c r="E34" t="n">
-        <v>268453806</v>
+        <v>270640348</v>
       </c>
       <c r="F34" t="n">
-        <v>6.45012</v>
+        <v>5.80717</v>
       </c>
     </row>
     <row r="35">
@@ -1269,16 +1269,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.044e-05</v>
+        <v>1.039e-05</v>
       </c>
       <c r="D35" t="n">
-        <v>4390443516</v>
+        <v>4365804086</v>
       </c>
       <c r="E35" t="n">
-        <v>841236763</v>
+        <v>852485531</v>
       </c>
       <c r="F35" t="n">
-        <v>9.43374</v>
+        <v>8.923859999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1293,16 +1293,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>221.68</v>
+        <v>221.87</v>
       </c>
       <c r="D36" t="n">
-        <v>4088138803</v>
+        <v>4086805671</v>
       </c>
       <c r="E36" t="n">
-        <v>66588918</v>
+        <v>64996379</v>
       </c>
       <c r="F36" t="n">
-        <v>0.09557</v>
+        <v>0.24147</v>
       </c>
     </row>
     <row r="37">
@@ -1317,16 +1317,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>27.75</v>
+        <v>27.73</v>
       </c>
       <c r="D37" t="n">
-        <v>3999969909</v>
+        <v>3996396949</v>
       </c>
       <c r="E37" t="n">
-        <v>20213299</v>
+        <v>17794008</v>
       </c>
       <c r="F37" t="n">
-        <v>0.90734</v>
+        <v>0.92908</v>
       </c>
     </row>
     <row r="38">
@@ -1341,16 +1341,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.37</v>
+        <v>3.36</v>
       </c>
       <c r="D38" t="n">
-        <v>3967644607</v>
+        <v>3957138556</v>
       </c>
       <c r="E38" t="n">
-        <v>227180722</v>
+        <v>227483967</v>
       </c>
       <c r="F38" t="n">
-        <v>5.26175</v>
+        <v>4.92774</v>
       </c>
     </row>
     <row r="39">
@@ -1365,16 +1365,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>260.77</v>
+        <v>260.45</v>
       </c>
       <c r="D39" t="n">
-        <v>3927946858</v>
+        <v>3924874399</v>
       </c>
       <c r="E39" t="n">
-        <v>386449541</v>
+        <v>386194759</v>
       </c>
       <c r="F39" t="n">
-        <v>5.655</v>
+        <v>5.74941</v>
       </c>
     </row>
     <row r="40">
@@ -1389,16 +1389,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6.34</v>
+        <v>6.31</v>
       </c>
       <c r="D40" t="n">
-        <v>3643819239</v>
+        <v>3630205661</v>
       </c>
       <c r="E40" t="n">
-        <v>331009471</v>
+        <v>331319334</v>
       </c>
       <c r="F40" t="n">
-        <v>4.07216</v>
+        <v>3.90311</v>
       </c>
     </row>
     <row r="41">
@@ -1413,64 +1413,64 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.068</v>
+        <v>1.062</v>
       </c>
       <c r="D41" t="n">
-        <v>3593507870</v>
+        <v>3569477708</v>
       </c>
       <c r="E41" t="n">
-        <v>106414261</v>
+        <v>106495921</v>
       </c>
       <c r="F41" t="n">
-        <v>4.34742</v>
+        <v>3.20128</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>tao</t>
+          <t>icp</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>433.33</v>
+        <v>7.37</v>
       </c>
       <c r="D42" t="n">
-        <v>3559938543</v>
+        <v>3538884457</v>
       </c>
       <c r="E42" t="n">
-        <v>217846340</v>
+        <v>90135187</v>
       </c>
       <c r="F42" t="n">
-        <v>13.27062</v>
+        <v>4.82233</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>icp</t>
+          <t>tao</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>7.41</v>
+        <v>431.42</v>
       </c>
       <c r="D43" t="n">
-        <v>3558632342</v>
+        <v>3536199927</v>
       </c>
       <c r="E43" t="n">
-        <v>105575995</v>
+        <v>221947991</v>
       </c>
       <c r="F43" t="n">
-        <v>5.19537</v>
+        <v>12.24481</v>
       </c>
     </row>
     <row r="44">
@@ -1485,16 +1485,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.999839</v>
+        <v>0.999786</v>
       </c>
       <c r="D44" t="n">
-        <v>3481604140</v>
+        <v>3481684031</v>
       </c>
       <c r="E44" t="n">
-        <v>200600798</v>
+        <v>202816119</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.00911</v>
+        <v>-0.0143</v>
       </c>
     </row>
     <row r="45">
@@ -1509,16 +1509,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>16.72</v>
+        <v>16.68</v>
       </c>
       <c r="D45" t="n">
-        <v>3344312866</v>
+        <v>3334898510</v>
       </c>
       <c r="E45" t="n">
-        <v>947284649</v>
+        <v>927414180</v>
       </c>
       <c r="F45" t="n">
-        <v>6.7373</v>
+        <v>4.89151</v>
       </c>
     </row>
     <row r="46">
@@ -1533,16 +1533,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.039</v>
+        <v>1.038</v>
       </c>
       <c r="D46" t="n">
-        <v>3251747767</v>
+        <v>3248904558</v>
       </c>
       <c r="E46" t="n">
-        <v>947198</v>
+        <v>805276</v>
       </c>
       <c r="F46" t="n">
-        <v>1.06598</v>
+        <v>0.43534</v>
       </c>
     </row>
     <row r="47">
@@ -1557,16 +1557,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>21.28</v>
+        <v>21.22</v>
       </c>
       <c r="D47" t="n">
-        <v>3207444572</v>
+        <v>3198232671</v>
       </c>
       <c r="E47" t="n">
-        <v>97620204</v>
+        <v>98369155</v>
       </c>
       <c r="F47" t="n">
-        <v>4.90565</v>
+        <v>4.18411</v>
       </c>
     </row>
     <row r="48">
@@ -1581,16 +1581,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>50.27</v>
+        <v>50</v>
       </c>
       <c r="D48" t="n">
-        <v>3018989610</v>
+        <v>2999139321</v>
       </c>
       <c r="E48" t="n">
-        <v>10356887</v>
+        <v>7582390</v>
       </c>
       <c r="F48" t="n">
-        <v>4.772</v>
+        <v>4.53236</v>
       </c>
     </row>
     <row r="49">
@@ -1605,16 +1605,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.03554456</v>
+        <v>0.03549073</v>
       </c>
       <c r="D49" t="n">
-        <v>2876899940</v>
+        <v>2872965327</v>
       </c>
       <c r="E49" t="n">
-        <v>54829505</v>
+        <v>54254949</v>
       </c>
       <c r="F49" t="n">
-        <v>8.8119</v>
+        <v>8.452389999999999</v>
       </c>
     </row>
     <row r="50">
@@ -1629,16 +1629,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>22.56</v>
+        <v>22.5</v>
       </c>
       <c r="D50" t="n">
-        <v>2839048446</v>
+        <v>2837124409</v>
       </c>
       <c r="E50" t="n">
-        <v>14792626</v>
+        <v>15074510</v>
       </c>
       <c r="F50" t="n">
-        <v>5.03251</v>
+        <v>4.45716</v>
       </c>
     </row>
     <row r="51">
@@ -1653,16 +1653,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.327816</v>
+        <v>0.327871</v>
       </c>
       <c r="D51" t="n">
-        <v>2800022733</v>
+        <v>2802557458</v>
       </c>
       <c r="E51" t="n">
-        <v>76845170</v>
+        <v>77237287</v>
       </c>
       <c r="F51" t="n">
-        <v>6.7772</v>
+        <v>6.57297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>